<commit_message>
archivos soporte diagrama deflujo
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Calidad/PTL_Checklist_procesos.xlsx
+++ b/qualtcom/Organizacional/Calidad/PTL_Checklist_procesos.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\escuela1\qualtcom\Organizacional\Calidad\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="588" windowWidth="15612" windowHeight="7092"/>
+    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <sheet name="Funcional" sheetId="5" r:id="rId5"/>
     <sheet name="No Conformidades" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -758,9 +763,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -776,6 +778,9 @@
     </xf>
     <xf numFmtId="165" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -799,6 +804,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -847,7 +855,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -882,7 +890,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1093,25 +1101,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="53.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.88671875" style="1" customWidth="1"/>
-    <col min="9" max="1024" width="11.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="1" customWidth="1"/>
+    <col min="9" max="1024" width="11.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="2" spans="1:6" ht="15.6">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="2"/>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
@@ -1119,7 +1127,7 @@
       <c r="E2" s="43"/>
       <c r="F2" s="43"/>
     </row>
-    <row r="4" spans="1:6" ht="15.6">
+    <row r="4" spans="1:6" ht="15.75">
       <c r="B4" s="42" t="s">
         <v>0</v>
       </c>
@@ -1139,7 +1147,7 @@
       <c r="E5" s="44"/>
       <c r="F5" s="44"/>
     </row>
-    <row r="6" spans="1:6" ht="13.8" customHeight="1">
+    <row r="6" spans="1:6" ht="13.9" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1275,7 +1283,7 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="19.5" customHeight="1"/>
-    <row r="22" spans="2:8" s="5" customFormat="1" ht="15.6">
+    <row r="22" spans="2:8" s="5" customFormat="1" ht="15.75">
       <c r="B22" s="42" t="s">
         <v>18</v>
       </c>
@@ -1297,7 +1305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="5" customFormat="1" ht="13.8">
+    <row r="24" spans="2:8" s="5" customFormat="1" ht="12.75">
       <c r="B24" s="8" t="s">
         <v>20</v>
       </c>
@@ -1310,7 +1318,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="2:8" s="5" customFormat="1" ht="13.8">
+    <row r="25" spans="2:8" s="5" customFormat="1" ht="12.75">
       <c r="B25" s="8" t="s">
         <v>21</v>
       </c>
@@ -1323,7 +1331,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="2:8" s="5" customFormat="1" ht="13.8">
+    <row r="26" spans="2:8" s="5" customFormat="1" ht="12.75">
       <c r="B26" s="8" t="s">
         <v>22</v>
       </c>
@@ -1336,14 +1344,14 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="2:8" s="5" customFormat="1" ht="13.8">
+    <row r="27" spans="2:8" s="5" customFormat="1" ht="12.75">
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
     </row>
-    <row r="28" spans="2:8" s="5" customFormat="1" ht="13.8" customHeight="1"/>
-    <row r="29" spans="2:8" s="5" customFormat="1" ht="14.4" customHeight="1">
+    <row r="28" spans="2:8" s="5" customFormat="1" ht="13.9" customHeight="1"/>
+    <row r="29" spans="2:8" s="5" customFormat="1" ht="14.45" customHeight="1">
       <c r="B29" s="42" t="s">
         <v>23</v>
       </c>
@@ -1351,7 +1359,7 @@
       <c r="D29" s="42"/>
       <c r="E29" s="14"/>
     </row>
-    <row r="30" spans="2:8" s="5" customFormat="1" ht="13.8">
+    <row r="30" spans="2:8" s="5" customFormat="1" ht="12.75">
       <c r="B30" s="6" t="s">
         <v>10</v>
       </c>
@@ -1363,7 +1371,7 @@
       </c>
       <c r="E30" s="15"/>
     </row>
-    <row r="31" spans="2:8" s="5" customFormat="1" ht="13.8">
+    <row r="31" spans="2:8" s="5" customFormat="1" ht="12.75">
       <c r="B31" s="8" t="s">
         <v>24</v>
       </c>
@@ -1377,7 +1385,7 @@
       </c>
       <c r="E31" s="15"/>
     </row>
-    <row r="32" spans="2:8" s="5" customFormat="1" ht="13.8">
+    <row r="32" spans="2:8" s="5" customFormat="1" ht="12.75">
       <c r="B32" s="8" t="s">
         <v>25</v>
       </c>
@@ -1390,7 +1398,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="2:4" s="5" customFormat="1" ht="13.8">
+    <row r="33" spans="2:4" s="5" customFormat="1" ht="12.75">
       <c r="B33" s="8" t="s">
         <v>22</v>
       </c>
@@ -1403,8 +1411,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="2:4" s="5" customFormat="1" ht="13.8"/>
-    <row r="35" spans="2:4" s="5" customFormat="1" ht="13.8"/>
+    <row r="34" spans="2:4" s="5" customFormat="1" ht="12.75"/>
+    <row r="35" spans="2:4" s="5" customFormat="1" ht="12.75"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B11:D11"/>
@@ -1432,17 +1440,17 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" style="17" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" style="17" customWidth="1"/>
     <col min="2" max="2" width="3" style="17" customWidth="1"/>
-    <col min="3" max="3" width="88.88671875" style="17" customWidth="1"/>
-    <col min="4" max="6" width="11.88671875" style="17" customWidth="1"/>
-    <col min="7" max="7" width="44.44140625" style="17" customWidth="1"/>
-    <col min="8" max="1024" width="11.88671875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="88.85546875" style="17" customWidth="1"/>
+    <col min="4" max="6" width="11.85546875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="44.42578125" style="17" customWidth="1"/>
+    <col min="8" max="1024" width="11.85546875" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:1024" ht="14.4" customHeight="1">
+    <row r="1" spans="3:1024" ht="14.45" customHeight="1">
       <c r="C1" s="45" t="s">
         <v>96</v>
       </c>
@@ -6615,13 +6623,13 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="17" customWidth="1"/>
-    <col min="2" max="2" width="96.21875" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.88671875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="44.44140625" style="17" customWidth="1"/>
-    <col min="7" max="1024" width="11.88671875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="96.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.85546875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="44.42578125" style="17" customWidth="1"/>
+    <col min="7" max="1024" width="11.85546875" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:1024">
@@ -38516,26 +38524,26 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="3" style="17" customWidth="1"/>
-    <col min="3" max="3" width="103.77734375" style="17" customWidth="1"/>
-    <col min="4" max="6" width="11.88671875" style="17" customWidth="1"/>
-    <col min="7" max="7" width="44.44140625" style="17" customWidth="1"/>
-    <col min="8" max="1024" width="11.88671875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="103.7109375" style="17" customWidth="1"/>
+    <col min="4" max="6" width="11.85546875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="44.42578125" style="17" customWidth="1"/>
+    <col min="8" max="1024" width="11.85546875" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:1024" customFormat="1" ht="14.4" customHeight="1">
-      <c r="B2" s="53"/>
-      <c r="C2" s="54" t="s">
+    <row r="2" spans="2:1024" customFormat="1" ht="14.45" customHeight="1">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58" t="s">
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="57" t="s">
         <v>61</v>
       </c>
       <c r="H2" s="17"/>
@@ -39557,8 +39565,8 @@
       <c r="AMJ2" s="17"/>
     </row>
     <row r="3" spans="2:1024" customFormat="1">
-      <c r="B3" s="53"/>
-      <c r="C3" s="54"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="53"/>
       <c r="D3" s="25" t="s">
         <v>62</v>
       </c>
@@ -39568,7 +39576,7 @@
       <c r="F3" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="58"/>
+      <c r="G3" s="57"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -40588,10 +40596,10 @@
       <c r="AMJ3" s="17"/>
     </row>
     <row r="4" spans="2:1024" customFormat="1">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="52"/>
+      <c r="C4" s="58"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="27"/>
@@ -41614,7 +41622,7 @@
       <c r="AMI4" s="17"/>
       <c r="AMJ4" s="17"/>
     </row>
-    <row r="5" spans="2:1024" customFormat="1" ht="27">
+    <row r="5" spans="2:1024" customFormat="1" ht="26.25">
       <c r="B5" s="28">
         <v>1</v>
       </c>
@@ -42643,7 +42651,7 @@
       <c r="AMI5" s="17"/>
       <c r="AMJ5" s="17"/>
     </row>
-    <row r="6" spans="2:1024" customFormat="1" ht="27">
+    <row r="6" spans="2:1024" customFormat="1" ht="26.25">
       <c r="B6" s="28">
         <v>2</v>
       </c>
@@ -43672,7 +43680,7 @@
       <c r="AMI6" s="17"/>
       <c r="AMJ6" s="17"/>
     </row>
-    <row r="7" spans="2:1024" customFormat="1" ht="27">
+    <row r="7" spans="2:1024" customFormat="1" ht="26.25">
       <c r="B7" s="28">
         <v>3</v>
       </c>
@@ -44702,10 +44710,10 @@
       <c r="AMJ7" s="17"/>
     </row>
     <row r="8" spans="2:1024" customFormat="1">
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="52"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
@@ -45777,10 +45785,10 @@
       <c r="G12" s="29"/>
     </row>
     <row r="13" spans="2:1024" s="31" customFormat="1">
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="52"/>
+      <c r="C13" s="58"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
       <c r="F13" s="27"/>
@@ -46075,6 +46083,11 @@
     <row r="208" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="C98:F98"/>
+    <mergeCell ref="C110:F110"/>
+    <mergeCell ref="C126:F126"/>
     <mergeCell ref="C54:F54"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -46086,11 +46099,6 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C33:F33"/>
     <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="C98:F98"/>
-    <mergeCell ref="C110:F110"/>
-    <mergeCell ref="C126:F126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -46106,33 +46114,33 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" style="17" customWidth="1"/>
     <col min="2" max="2" width="3" style="17" customWidth="1"/>
-    <col min="3" max="3" width="74.109375" style="17" customWidth="1"/>
-    <col min="4" max="6" width="11.88671875" style="17" customWidth="1"/>
-    <col min="7" max="7" width="44.44140625" style="17" customWidth="1"/>
-    <col min="8" max="1024" width="11.88671875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="74.140625" style="17" customWidth="1"/>
+    <col min="4" max="6" width="11.85546875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="44.42578125" style="17" customWidth="1"/>
+    <col min="8" max="1024" width="11.85546875" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:1024" ht="14.4" customHeight="1">
-      <c r="B2" s="53"/>
-      <c r="C2" s="54" t="s">
+    <row r="2" spans="2:1024" ht="14.45" customHeight="1">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58" t="s">
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="57" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="3" spans="2:1024">
-      <c r="B3" s="53"/>
-      <c r="C3" s="54"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="53"/>
       <c r="D3" s="25" t="s">
         <v>62</v>
       </c>
@@ -46142,13 +46150,13 @@
       <c r="F3" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="58"/>
+      <c r="G3" s="57"/>
     </row>
     <row r="4" spans="2:1024">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="52"/>
+      <c r="C4" s="58"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="27"/>
@@ -46203,10 +46211,10 @@
       <c r="G8" s="36"/>
     </row>
     <row r="9" spans="2:1024" customFormat="1">
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="52"/>
+      <c r="C9" s="58"/>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
       <c r="F9" s="26"/>
@@ -53428,10 +53436,10 @@
       <c r="AMJ17" s="17"/>
     </row>
     <row r="18" spans="2:1024" s="31" customFormat="1">
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="52"/>
+      <c r="C18" s="58"/>
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
@@ -53759,12 +53767,6 @@
     <row r="222" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="C99:F99"/>
     <mergeCell ref="C111:F111"/>
     <mergeCell ref="C127:F127"/>
@@ -53774,6 +53776,12 @@
     <mergeCell ref="C55:F55"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="C76:F76"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -53785,21 +53793,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="2" max="2" width="2.88671875" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="42" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" customWidth="1"/>
-    <col min="8" max="8" width="27.33203125" customWidth="1"/>
-    <col min="9" max="1024" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1"/>
+    <col min="9" max="1024" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="15.6" customHeight="1">
@@ -53822,7 +53830,7 @@
       <c r="G4" s="60"/>
       <c r="H4" s="60"/>
     </row>
-    <row r="5" spans="2:8" ht="28.8">
+    <row r="5" spans="2:8" ht="30">
       <c r="B5" s="41" t="s">
         <v>90</v>
       </c>

</xml_diff>